<commit_message>
MAJ plan afficheur temp
</commit_message>
<xml_diff>
--- a/EL - Electrical/Autre/Carte avant/Lien mcp - 7 segements.xlsx
+++ b/EL - Electrical/Autre/Carte avant/Lien mcp - 7 segements.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D00F39-D739-4308-AB23-FD31AB2B2603}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60C39C3-2030-4E57-8F32-7AFB35364D72}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,10 +535,10 @@
         <v>4</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -558,10 +558,10 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -715,10 +715,10 @@
         <v>14</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="7:10" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>